<commit_message>
updated values for unet in confronto_modelli
</commit_message>
<xml_diff>
--- a/confronto_modelli.xlsx
+++ b/confronto_modelli.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescobaraldi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescobaraldi/Desktop/deep-seasonal-color-analysis-system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CEF87B-0FA3-4145-BE02-4DD84C0C55DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A968C1AB-4661-7841-BDD2-057712D5BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{9A0420F9-B2E0-4BE6-8135-95C011EC091E}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Unet</t>
   </si>
   <si>
-    <t>4.72</t>
-  </si>
-  <si>
     <t>Deeplabv3</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>0.160</t>
+  </si>
+  <si>
+    <t>6.1</t>
   </si>
 </sst>
 </file>
@@ -823,7 +823,7 @@
   <dimension ref="B1:J5"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>5</v>
@@ -872,7 +872,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="7">
         <v>69</v>
@@ -881,16 +881,16 @@
         <v>6266</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="J3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3">
         <v>66</v>
@@ -908,16 +908,16 @@
         <v>947</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="J4" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -926,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="12">
         <v>53</v>
@@ -935,16 +935,16 @@
         <v>5023</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="J5" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +961,7 @@
   <dimension ref="B1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>5</v>
@@ -1010,31 +1010,31 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E3" s="7">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7">
         <v>8997</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21"/>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>

</xml_diff>

<commit_message>
added results of training demo for deeplab
</commit_message>
<xml_diff>
--- a/confronto_modelli.xlsx
+++ b/confronto_modelli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescobaraldi/Desktop/deep-seasonal-color-analysis-system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A797F1-0334-E942-B627-30D1428B9BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522129A7-15B3-4C4D-9C7C-6D8ADC2E2568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-100" windowWidth="38400" windowHeight="21100" xr2:uid="{9A0420F9-B2E0-4BE6-8135-95C011EC091E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{9A0420F9-B2E0-4BE6-8135-95C011EC091E}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Modello</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>6.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -822,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2786497-5FEA-42EE-990D-21E7E369B036}">
   <dimension ref="B1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -960,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BD8A06-57BD-4949-ADCC-3313E00C4CC6}">
   <dimension ref="B1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,13 +1042,27 @@
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="15"/>
+      <c r="D4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="12">
+        <v>14136</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update confronto_modelli.xlsx with deeplab test results
</commit_message>
<xml_diff>
--- a/confronto_modelli.xlsx
+++ b/confronto_modelli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescobaraldi/Desktop/deep-seasonal-color-analysis-system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522129A7-15B3-4C4D-9C7C-6D8ADC2E2568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC898C23-62D3-403E-B88A-FBE32B076552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{9A0420F9-B2E0-4BE6-8135-95C011EC091E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9A0420F9-B2E0-4BE6-8135-95C011EC091E}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="1" r:id="rId1"/>
@@ -21,20 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Modello</t>
   </si>
@@ -138,7 +130,16 @@
     <t>10.2</t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>0.746</t>
+  </si>
+  <si>
+    <t>0.728</t>
+  </si>
+  <si>
+    <t>0.457</t>
+  </si>
+  <si>
+    <t>0.166</t>
   </si>
 </sst>
 </file>
@@ -513,8 +514,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -530,7 +531,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -832,20 +833,20 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="8" t="s">
@@ -870,7 +871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -899,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20"/>
       <c r="C4" s="18" t="s">
         <v>8</v>
@@ -926,7 +927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21"/>
       <c r="C5" s="5" t="s">
         <v>9</v>
@@ -967,23 +968,23 @@
   <dimension ref="B1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="8" t="s">
@@ -1008,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="21"/>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -1045,8 +1046,8 @@
       <c r="D4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>34</v>
+      <c r="E4" s="12">
+        <v>89</v>
       </c>
       <c r="F4" s="12">
         <v>14136</v>
@@ -1055,13 +1056,13 @@
         <v>34</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>